<commit_message>
Enhance workflow automation by adding a new batch script for GTS submission, which automates the process of filling out GTS forms. Update the `.gitignore` to exclude test data reports and logs. Modify the `config.yaml` for improved configuration management and logging. Refactor the `GTSSubmitter` class to allow the browser to remain open for user interaction after submission cancellation. Update the `README.md` to document new features and configuration options for the Mole automation tool.
</commit_message>
<xml_diff>
--- a/automation/auto-vpo/input/GTS_Submit.xlsx
+++ b/automation/auto-vpo/input/GTS_Submit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/qibai_chen_intel_com/Documents/Documents/AI_Code/automation/auto-vpo/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_F25DC773A252ABDACC10483D099D7C465BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB9ECD4B-4A33-4CD5-9056-FC7706565219}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_F25DC773A252ABDACC10483D099D7C465BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2394261A-756F-49E5-B5EC-AE0ED0B58B7D}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="4392" windowWidth="23040" windowHeight="12168" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="2660" windowWidth="28800" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,16 +60,16 @@
     <t>needed?</t>
   </si>
   <si>
-    <t>12Hr</t>
+    <t>WW52.2</t>
   </si>
   <si>
-    <t>WW51.3</t>
+    <t>48Hr</t>
   </si>
   <si>
-    <t>2PM-2AM</t>
+    <t>5PM-5PM</t>
   </si>
   <si>
-    <t>HDMX2524_LEVEL4/5</t>
+    <t>HDMX2524_LEVEL4</t>
   </si>
 </sst>
 </file>
@@ -1399,22 +1399,22 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="31.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="31.36328125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" ht="29">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1468,10 +1468,10 @@
         <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update automation scripts and configuration for improved functionality and logging. Added new log files to `.gitignore`, modified batch scripts for GTS submission to reflect updated file paths, and enhanced error handling in the workflow automation process. Updated `config.yaml` for better configuration management and added support for new directory structures in data processing. Removed obsolete files and improved logging details for better traceability during execution.
</commit_message>
<xml_diff>
--- a/automation/auto-vpo/input/GTS_Submit.xlsx
+++ b/automation/auto-vpo/input/GTS_Submit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/qibai_chen_intel_com/Documents/Documents/AI_Code/automation/auto-vpo/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="11_F25DC773A252ABDACC10483D099D7C465BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2394261A-756F-49E5-B5EC-AE0ED0B58B7D}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_F25DC773A252ABDACC10483D099D7C465BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C48ADA39-4B5E-402C-8561-38A510986F70}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2660" windowWidth="28800" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12110" yWindow="2490" windowWidth="23060" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,16 +60,16 @@
     <t>needed?</t>
   </si>
   <si>
-    <t>WW52.2</t>
-  </si>
-  <si>
     <t>48Hr</t>
   </si>
   <si>
-    <t>5PM-5PM</t>
+    <t>HDMX2524_LEVEL4</t>
   </si>
   <si>
-    <t>HDMX2524_LEVEL4</t>
+    <t>WW1.1</t>
+  </si>
+  <si>
+    <t>12PM-12PM</t>
   </si>
 </sst>
 </file>
@@ -1399,7 +1399,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.36328125" defaultRowHeight="14.5"/>
@@ -1462,16 +1462,16 @@
       <c r="C3" s="5"/>
       <c r="D3" s="4"/>
       <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>